<commit_message>
back to the default face
</commit_message>
<xml_diff>
--- a/face detection/static/face_details.xlsx
+++ b/face detection/static/face_details.xlsx
@@ -453,15 +453,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>(115, 14, 31, 41)</t>
+          <t>(98, 197, 431, 573)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9997079968452454</v>
+        <v>0.9999836683273315</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'left_eye': (122, 30), 'right_eye': (138, 29), 'nose': (130, 39), 'mouth_left': (122, 44), 'mouth_right': (138, 43)}</t>
+          <t>{'left_eye': (238, 425), 'right_eye': (439, 468), 'nose': (322, 577), 'mouth_left': (201, 598), 'mouth_right': (393, 642)}</t>
         </is>
       </c>
     </row>

</xml_diff>